<commit_message>
Editing existing test cases
</commit_message>
<xml_diff>
--- a/Movie_Name.xlsx
+++ b/Movie_Name.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>S.NO.</t>
   </si>
@@ -20,25 +20,94 @@
     <t>Movie Names whose ContentAvailable is 0</t>
   </si>
   <si>
+    <t>K.G.F. Chapter 2</t>
+  </si>
+  <si>
+    <t>Thalaivi</t>
+  </si>
+  <si>
+    <t>F9: The Fast Saga</t>
+  </si>
+  <si>
+    <t>Top Gun: Maverick</t>
+  </si>
+  <si>
+    <t>Wonder Woman 1984</t>
+  </si>
+  <si>
+    <t>Black Widow</t>
+  </si>
+  <si>
+    <t>No Time To Die</t>
+  </si>
+  <si>
     <t>Bunty Aur Babli 2</t>
   </si>
   <si>
+    <t>Shershaah</t>
+  </si>
+  <si>
+    <t>Tenet</t>
+  </si>
+  <si>
+    <t>Jungle Cruise</t>
+  </si>
+  <si>
+    <t>Shamshera</t>
+  </si>
+  <si>
+    <t>Bhool Bhulaiya 2</t>
+  </si>
+  <si>
+    <t>Morbius</t>
+  </si>
+  <si>
+    <t>Gangubai Kathiawadi</t>
+  </si>
+  <si>
     <t>Haseen Dillruba</t>
   </si>
   <si>
+    <t>Rambo</t>
+  </si>
+  <si>
+    <t>Toofan</t>
+  </si>
+  <si>
+    <t>Satyameva Jayate 2</t>
+  </si>
+  <si>
     <t>The Big Bull</t>
   </si>
   <si>
+    <t>Prithviraj</t>
+  </si>
+  <si>
     <t>Maidaan</t>
   </si>
   <si>
+    <t>Laal Singh Chaddha</t>
+  </si>
+  <si>
     <t>Mr. Lele</t>
   </si>
   <si>
+    <t>Bachchan Pandey</t>
+  </si>
+  <si>
     <t>Shabaash Mithu</t>
   </si>
   <si>
+    <t>Bell Bottom</t>
+  </si>
+  <si>
     <t>Heropanti 2</t>
+  </si>
+  <si>
+    <t>Takht</t>
+  </si>
+  <si>
+    <t>Black Adam</t>
   </si>
 </sst>
 </file>
@@ -83,7 +152,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -153,6 +222,190 @@
         <v>8</v>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="B12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="B13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>13.0</v>
+      </c>
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="B15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="B16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>16.0</v>
+      </c>
+      <c r="B17" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>17.0</v>
+      </c>
+      <c r="B18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="B19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>19.0</v>
+      </c>
+      <c r="B20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="B21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="B22" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>22.0</v>
+      </c>
+      <c r="B23" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>23.0</v>
+      </c>
+      <c r="B24" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>24.0</v>
+      </c>
+      <c r="B25" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>25.0</v>
+      </c>
+      <c r="B26" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>26.0</v>
+      </c>
+      <c r="B27" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>27.0</v>
+      </c>
+      <c r="B28" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>28.0</v>
+      </c>
+      <c r="B29" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>29.0</v>
+      </c>
+      <c r="B30" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="B31" t="s">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>